<commit_message>
BurndownChart - Sprint 2 Updated
</commit_message>
<xml_diff>
--- a/Project/Phase_2/Sprint2/Burndown-Chart.xlsx
+++ b/Project/Phase_2/Sprint2/Burndown-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utilizador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCFEA72-9B5B-4D59-BE16-3F304FD73A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F025FD5C-5871-4F5B-8AC3-9BB6DB413C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{81909052-7909-4177-A7BE-AF9923893C7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Ideal Burndown</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Completed Effort</t>
-  </si>
-  <si>
-    <t>Day 9</t>
   </si>
   <si>
     <t>Day 8</t>
@@ -199,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -455,17 +452,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -521,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,9 +531,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,19 +585,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,7 +775,7 @@
             <c:strRef>
               <c:f>'Burndown Chart'!$D$5:$M$5</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 0</c:v>
                 </c:pt>
@@ -819,9 +802,6 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -857,9 +837,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -929,7 +906,7 @@
             <c:strRef>
               <c:f>'Burndown Chart'!$D$5:$M$5</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 0</c:v>
                 </c:pt>
@@ -956,9 +933,6 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -994,9 +968,6 @@
                   <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>56.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1039,7 +1010,7 @@
             <c:strRef>
               <c:f>'Burndown Chart'!$D$5:$M$5</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 0</c:v>
                 </c:pt>
@@ -1066,9 +1037,6 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1083,30 +1051,27 @@
                   <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.222222222222221</c:v>
+                  <c:v>49.4375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.944444444444443</c:v>
+                  <c:v>42.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.666666666666671</c:v>
+                  <c:v>35.3125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.388888888888889</c:v>
+                  <c:v>28.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.111111111111111</c:v>
+                  <c:v>21.1875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.833333333333336</c:v>
+                  <c:v>14.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.555555555555557</c:v>
+                  <c:v>7.0625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2777777777777786</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1925,15 +1890,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2158688</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>2480</xdr:rowOff>
+      <xdr:colOff>2188571</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>686175</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>44171</xdr:rowOff>
+      <xdr:colOff>716058</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>74054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2258,409 +2223,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FC3085-A52E-45A9-AAEC-F19CACED0953}">
-  <dimension ref="B1:N23"/>
+  <dimension ref="B1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="33" t="s">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="37"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6">
+        <v>44874</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44875</v>
+      </c>
+      <c r="G4" s="4">
+        <v>44876</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44877</v>
+      </c>
+      <c r="I4" s="4">
+        <v>44878</v>
+      </c>
+      <c r="J4" s="4">
+        <v>44879</v>
+      </c>
+      <c r="K4" s="5">
+        <v>44880</v>
+      </c>
+      <c r="L4" s="4">
+        <v>44881</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="25">
+        <v>1</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="35"/>
+      <c r="D6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="38"/>
+    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="26">
+        <v>2</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9">
+        <v>15</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="21"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+    <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="26">
+        <v>3</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9">
         <v>15</v>
       </c>
-      <c r="C4" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6">
-        <v>44865</v>
-      </c>
-      <c r="F4" s="4">
-        <v>44866</v>
-      </c>
-      <c r="G4" s="4">
-        <v>44867</v>
-      </c>
-      <c r="H4" s="4">
-        <v>44868</v>
-      </c>
-      <c r="I4" s="4">
-        <v>44869</v>
-      </c>
-      <c r="J4" s="4">
-        <v>44870</v>
-      </c>
-      <c r="K4" s="5">
-        <v>44871</v>
-      </c>
-      <c r="L4" s="4">
-        <v>44872</v>
-      </c>
-      <c r="M4" s="4">
-        <v>44873</v>
-      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="21"/>
     </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
+    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="26">
+        <v>4</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="26">
+        <v>5</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="26">
+        <v>6</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9">
         <v>10</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="31">
         <v>7</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="9">
+        <v>10</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="21"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="26">
-        <v>1</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="27">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="10">
-        <v>15</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="27">
-        <v>3</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="10">
-        <v>15</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-    </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="27">
-        <v>4</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="10">
-        <v>5</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="27">
-        <v>5</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="27">
-        <v>6</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="10">
-        <v>10</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="32">
-        <v>7</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="10">
-        <v>10</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="16">
+      <c r="C13" s="39"/>
+      <c r="D13" s="15">
         <v>0</v>
       </c>
-      <c r="E13" s="17">
-        <f t="shared" ref="E13:M13" ca="1" si="0">SUM(E11:E20)</f>
+      <c r="E13" s="16">
+        <f t="shared" ref="E13:L13" ca="1" si="0">SUM(E11:E20)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M13" s="16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="43" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="11">
+      <c r="C14" s="43"/>
+      <c r="D14" s="10">
         <f>SUM(D6:D13)</f>
         <v>56.5</v>
       </c>
-      <c r="E14" s="12">
-        <f t="shared" ref="E14:M14" si="1">D14-SUM(E6:E12)</f>
+      <c r="E14" s="11">
+        <f t="shared" ref="E14:L14" si="1">D14-SUM(E6:E12)</f>
         <v>56.5</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="11">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="M14" s="12">
-        <f t="shared" si="1"/>
-        <v>56.5</v>
-      </c>
-      <c r="N14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="41" t="s">
+    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="13">
+      <c r="C15" s="41"/>
+      <c r="D15" s="12">
         <f>D14</f>
         <v>56.5</v>
       </c>
-      <c r="E15" s="14">
-        <f>$D$15-($D$15/9*1)</f>
-        <v>50.222222222222221</v>
-      </c>
-      <c r="F15" s="14">
-        <f>$D$15-($D$15/9*2)</f>
-        <v>43.944444444444443</v>
-      </c>
-      <c r="G15" s="14">
-        <f>$D$15-($D$15/9*3)</f>
-        <v>37.666666666666671</v>
-      </c>
-      <c r="H15" s="14">
-        <f>$D$15-($D$15/9*4)</f>
-        <v>31.388888888888889</v>
-      </c>
-      <c r="I15" s="14">
-        <f>$D$15-($D$15/9*5)</f>
-        <v>25.111111111111111</v>
-      </c>
-      <c r="J15" s="14">
-        <f>$D$15-($D$15/9*6)</f>
-        <v>18.833333333333336</v>
-      </c>
-      <c r="K15" s="14">
-        <f>$D$15-($D$15/9*7)</f>
-        <v>12.555555555555557</v>
-      </c>
-      <c r="L15" s="15">
-        <f>$D$15-($D$15/9*8)</f>
-        <v>6.2777777777777786</v>
-      </c>
-      <c r="M15" s="9">
-        <f>$D$15-($D$15/9*9)</f>
+      <c r="E15" s="13">
+        <f t="shared" ref="E15:L15" si="2">$D$15-($D$15/COLUMNS(E6:L6)*E16)</f>
+        <v>49.4375</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="2"/>
+        <v>42.375</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="2"/>
+        <v>35.3125</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="2"/>
+        <v>28.25</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="2"/>
+        <v>21.1875</v>
+      </c>
+      <c r="J15" s="13">
+        <f t="shared" si="2"/>
+        <v>14.125</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="2"/>
+        <v>7.0625</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>E16 +1</f>
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:L16" si="3">F16 +1</f>
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
     <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B14:C14"/>

</xml_diff>